<commit_message>
Menus done + A series done
TODO: bugfixes + B-E series of tracks
</commit_message>
<xml_diff>
--- a/levelPlotter.xlsx
+++ b/levelPlotter.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zycai\Desktop\Create\Programming\RocketRacer\tracks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zycai\Desktop\Create\Programming\RocketRacer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0C4064-D9CC-4738-81D6-2A91507F41EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A65CB-600F-4149-961C-A0177F5E90B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{0AA58C0D-6055-4E5C-B55F-20E05DAE3D88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{0AA58C0D-6055-4E5C-B55F-20E05DAE3D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Grid" sheetId="1" r:id="rId1"/>
     <sheet name="A01" sheetId="2" r:id="rId2"/>
     <sheet name="A02" sheetId="4" r:id="rId3"/>
     <sheet name="A03" sheetId="5" r:id="rId4"/>
+    <sheet name="A04" sheetId="8" r:id="rId5"/>
+    <sheet name="A05" sheetId="7" r:id="rId6"/>
+    <sheet name="B01" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="7">
   <si>
     <t>w</t>
   </si>
@@ -113,7 +116,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="77">
     <dxf>
       <fill>
         <patternFill>
@@ -215,6 +218,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -313,6 +358,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -320,6 +407,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
@@ -327,6 +449,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -334,6 +491,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -341,6 +533,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -348,6 +575,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -355,91 +617,42 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -756,7 +969,7 @@
   <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AH34"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,26 +1325,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AG33">
-    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="76" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="2" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="74" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="4" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="72" priority="5" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="71" priority="6" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="7" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="70" priority="7" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="C">
-      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1144,7 +1357,7 @@
   <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AN9" sqref="AN9"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,25 +1764,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AG33">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="69" priority="1" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="68" priority="2" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="67" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="66" priority="4" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="64" priority="6" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="63" priority="7" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1582,7 +1795,7 @@
   <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17:J18"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,53 +1904,227 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
       <c r="AH2" s="1"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
       <c r="AH3" s="1"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
       <c r="AH4" s="1"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
       <c r="AH5" s="1"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
       <c r="AH6" s="1"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
+      </c>
       <c r="AH7" s="1"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
       <c r="AH8" s="1"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
       <c r="AH9" s="1"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>0</v>
       </c>
       <c r="AH10" s="1"/>
     </row>
@@ -1916,26 +2303,49 @@
       <c r="AH34" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AG33">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="C">
+  <conditionalFormatting sqref="L2:AG7 B8:AG33">
+    <cfRule type="containsText" dxfId="62" priority="8" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="61" priority="9" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="60" priority="10" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="59" priority="11" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="58" priority="12" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="6" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="57" priority="13" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="56" priority="14" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:K7">
+    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="4" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="5" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="6" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1948,8 +2358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8D00D1-7515-4EBB-9F3C-45EFE8B90C60}">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,12 +2492,99 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>0</v>
+      </c>
       <c r="AH6" s="1"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
@@ -2164,6 +2661,9 @@
         <v>0</v>
       </c>
       <c r="AD7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="s">
         <v>0</v>
       </c>
       <c r="AH7" s="1"/>
@@ -2172,19 +2672,25 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
       <c r="E8" t="s">
         <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4</v>
       </c>
       <c r="L8" t="s">
         <v>6</v>
       </c>
+      <c r="S8" t="s">
+        <v>4</v>
+      </c>
       <c r="W8" t="s">
         <v>6</v>
       </c>
       <c r="AD8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="s">
         <v>0</v>
       </c>
       <c r="AH8" s="1"/>
@@ -2193,6 +2699,9 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
@@ -2233,6 +2742,9 @@
         <v>0</v>
       </c>
       <c r="AD9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="s">
         <v>0</v>
       </c>
       <c r="AH9" s="1"/>
@@ -2241,9 +2753,15 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
       <c r="I10" t="s">
         <v>0</v>
       </c>
@@ -2298,7 +2816,13 @@
       <c r="Z10" t="s">
         <v>0</v>
       </c>
+      <c r="AA10" t="s">
+        <v>3</v>
+      </c>
       <c r="AD10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="s">
         <v>0</v>
       </c>
       <c r="AH10" s="1"/>
@@ -2307,6 +2831,9 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
@@ -2328,36 +2855,6 @@
       <c r="L11" t="s">
         <v>0</v>
       </c>
-      <c r="M11" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" t="s">
-        <v>0</v>
-      </c>
-      <c r="T11" t="s">
-        <v>0</v>
-      </c>
-      <c r="U11" t="s">
-        <v>0</v>
-      </c>
-      <c r="V11" t="s">
-        <v>0</v>
-      </c>
       <c r="W11" t="s">
         <v>0</v>
       </c>
@@ -2377,6 +2874,9 @@
         <v>3</v>
       </c>
       <c r="AD11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="s">
         <v>0</v>
       </c>
       <c r="AH11" s="1"/>
@@ -2385,6 +2885,9 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
@@ -2394,54 +2897,6 @@
       <c r="I12" t="s">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
-        <v>0</v>
-      </c>
-      <c r="S12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
-        <v>0</v>
-      </c>
-      <c r="U12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" t="s">
-        <v>0</v>
-      </c>
-      <c r="W12" t="s">
-        <v>0</v>
-      </c>
-      <c r="X12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>0</v>
-      </c>
       <c r="Z12" t="s">
         <v>0</v>
       </c>
@@ -2449,6 +2904,9 @@
         <v>0</v>
       </c>
       <c r="AD12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="s">
         <v>0</v>
       </c>
       <c r="AH12" s="1"/>
@@ -2457,6 +2915,9 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
@@ -2466,54 +2927,6 @@
       <c r="I13" t="s">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>0</v>
-      </c>
-      <c r="R13" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" t="s">
-        <v>0</v>
-      </c>
-      <c r="T13" t="s">
-        <v>0</v>
-      </c>
-      <c r="U13" t="s">
-        <v>0</v>
-      </c>
-      <c r="V13" t="s">
-        <v>0</v>
-      </c>
-      <c r="W13" t="s">
-        <v>0</v>
-      </c>
-      <c r="X13" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>0</v>
-      </c>
       <c r="Z13" t="s">
         <v>0</v>
       </c>
@@ -2521,6 +2934,9 @@
         <v>0</v>
       </c>
       <c r="AD13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="s">
         <v>0</v>
       </c>
       <c r="AH13" s="1"/>
@@ -2529,6 +2945,9 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
@@ -2538,60 +2957,6 @@
       <c r="H14" t="s">
         <v>0</v>
       </c>
-      <c r="I14" t="s">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
-        <v>0</v>
-      </c>
-      <c r="M14" t="s">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" t="s">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>0</v>
-      </c>
-      <c r="R14" t="s">
-        <v>0</v>
-      </c>
-      <c r="S14" t="s">
-        <v>0</v>
-      </c>
-      <c r="T14" t="s">
-        <v>0</v>
-      </c>
-      <c r="U14" t="s">
-        <v>0</v>
-      </c>
-      <c r="V14" t="s">
-        <v>0</v>
-      </c>
-      <c r="W14" t="s">
-        <v>0</v>
-      </c>
-      <c r="X14" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>0</v>
-      </c>
       <c r="AA14" t="s">
         <v>0</v>
       </c>
@@ -2599,6 +2964,9 @@
         <v>0</v>
       </c>
       <c r="AD14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="s">
         <v>0</v>
       </c>
       <c r="AH14" s="1"/>
@@ -2607,6 +2975,9 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
       <c r="E15" t="s">
         <v>0</v>
       </c>
@@ -2616,60 +2987,6 @@
       <c r="H15" t="s">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>0</v>
-      </c>
-      <c r="R15" t="s">
-        <v>0</v>
-      </c>
-      <c r="S15" t="s">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
-        <v>0</v>
-      </c>
-      <c r="U15" t="s">
-        <v>0</v>
-      </c>
-      <c r="V15" t="s">
-        <v>0</v>
-      </c>
-      <c r="W15" t="s">
-        <v>0</v>
-      </c>
-      <c r="X15" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>0</v>
-      </c>
       <c r="AA15" t="s">
         <v>0</v>
       </c>
@@ -2677,6 +2994,9 @@
         <v>0</v>
       </c>
       <c r="AD15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="s">
         <v>0</v>
       </c>
       <c r="AH15" s="1"/>
@@ -2685,6 +3005,9 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
@@ -2697,60 +3020,6 @@
       <c r="H16" t="s">
         <v>0</v>
       </c>
-      <c r="I16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" t="s">
-        <v>0</v>
-      </c>
-      <c r="T16" t="s">
-        <v>0</v>
-      </c>
-      <c r="U16" t="s">
-        <v>0</v>
-      </c>
-      <c r="V16" t="s">
-        <v>0</v>
-      </c>
-      <c r="W16" t="s">
-        <v>0</v>
-      </c>
-      <c r="X16" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>0</v>
-      </c>
       <c r="AA16" t="s">
         <v>0</v>
       </c>
@@ -2758,6 +3027,9 @@
         <v>0</v>
       </c>
       <c r="AD16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE16" t="s">
         <v>0</v>
       </c>
       <c r="AH16" s="1"/>
@@ -2766,6 +3038,9 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
@@ -2775,60 +3050,6 @@
       <c r="H17" t="s">
         <v>0</v>
       </c>
-      <c r="I17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" t="s">
-        <v>0</v>
-      </c>
-      <c r="S17" t="s">
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
-        <v>0</v>
-      </c>
-      <c r="U17" t="s">
-        <v>0</v>
-      </c>
-      <c r="V17" t="s">
-        <v>0</v>
-      </c>
-      <c r="W17" t="s">
-        <v>0</v>
-      </c>
-      <c r="X17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>0</v>
-      </c>
       <c r="AA17" t="s">
         <v>0</v>
       </c>
@@ -2836,6 +3057,9 @@
         <v>0</v>
       </c>
       <c r="AD17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="s">
         <v>0</v>
       </c>
       <c r="AH17" s="1"/>
@@ -2844,6 +3068,9 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
@@ -2853,60 +3080,6 @@
       <c r="H18" t="s">
         <v>0</v>
       </c>
-      <c r="I18" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>0</v>
-      </c>
-      <c r="R18" t="s">
-        <v>0</v>
-      </c>
-      <c r="S18" t="s">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>0</v>
-      </c>
-      <c r="U18" t="s">
-        <v>0</v>
-      </c>
-      <c r="V18" t="s">
-        <v>0</v>
-      </c>
-      <c r="W18" t="s">
-        <v>0</v>
-      </c>
-      <c r="X18" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>0</v>
-      </c>
       <c r="AA18" t="s">
         <v>0</v>
       </c>
@@ -2914,6 +3087,9 @@
         <v>0</v>
       </c>
       <c r="AD18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="s">
         <v>0</v>
       </c>
       <c r="AH18" s="1"/>
@@ -2922,6 +3098,9 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
       <c r="E19" t="s">
         <v>0</v>
       </c>
@@ -2931,60 +3110,6 @@
       <c r="H19" t="s">
         <v>0</v>
       </c>
-      <c r="I19" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" t="s">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>0</v>
-      </c>
-      <c r="R19" t="s">
-        <v>0</v>
-      </c>
-      <c r="S19" t="s">
-        <v>0</v>
-      </c>
-      <c r="T19" t="s">
-        <v>0</v>
-      </c>
-      <c r="U19" t="s">
-        <v>0</v>
-      </c>
-      <c r="V19" t="s">
-        <v>0</v>
-      </c>
-      <c r="W19" t="s">
-        <v>0</v>
-      </c>
-      <c r="X19" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>0</v>
-      </c>
       <c r="AA19" t="s">
         <v>0</v>
       </c>
@@ -2992,6 +3117,9 @@
         <v>0</v>
       </c>
       <c r="AD19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="s">
         <v>0</v>
       </c>
       <c r="AH19" s="1"/>
@@ -3000,6 +3128,9 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
       <c r="E20" t="s">
         <v>0</v>
       </c>
@@ -3009,70 +3140,16 @@
       <c r="H20" t="s">
         <v>0</v>
       </c>
-      <c r="I20" t="s">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" t="s">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>0</v>
-      </c>
-      <c r="M20" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" t="s">
-        <v>0</v>
-      </c>
-      <c r="O20" t="s">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>0</v>
-      </c>
-      <c r="R20" t="s">
-        <v>0</v>
-      </c>
-      <c r="S20" t="s">
-        <v>0</v>
-      </c>
-      <c r="T20" t="s">
-        <v>0</v>
-      </c>
-      <c r="U20" t="s">
-        <v>0</v>
-      </c>
-      <c r="V20" t="s">
-        <v>0</v>
-      </c>
-      <c r="W20" t="s">
-        <v>0</v>
-      </c>
-      <c r="X20" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>0</v>
-      </c>
       <c r="AA20" t="s">
         <v>0</v>
       </c>
       <c r="AB20" t="s">
         <v>0</v>
       </c>
-      <c r="AC20" t="s">
-        <v>4</v>
-      </c>
       <c r="AD20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE20" t="s">
         <v>0</v>
       </c>
       <c r="AH20" s="1"/>
@@ -3081,6 +3158,9 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
       <c r="E21" t="s">
         <v>0</v>
       </c>
@@ -3090,60 +3170,6 @@
       <c r="H21" t="s">
         <v>0</v>
       </c>
-      <c r="I21" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M21" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" t="s">
-        <v>0</v>
-      </c>
-      <c r="O21" t="s">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>0</v>
-      </c>
-      <c r="R21" t="s">
-        <v>0</v>
-      </c>
-      <c r="S21" t="s">
-        <v>0</v>
-      </c>
-      <c r="T21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U21" t="s">
-        <v>0</v>
-      </c>
-      <c r="V21" t="s">
-        <v>0</v>
-      </c>
-      <c r="W21" t="s">
-        <v>0</v>
-      </c>
-      <c r="X21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>0</v>
-      </c>
       <c r="AA21" t="s">
         <v>0</v>
       </c>
@@ -3151,6 +3177,9 @@
         <v>0</v>
       </c>
       <c r="AD21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="s">
         <v>0</v>
       </c>
       <c r="AH21" s="1"/>
@@ -3159,6 +3188,9 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
       <c r="E22" t="s">
         <v>0</v>
       </c>
@@ -3168,60 +3200,6 @@
       <c r="H22" t="s">
         <v>0</v>
       </c>
-      <c r="I22" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>0</v>
-      </c>
-      <c r="M22" t="s">
-        <v>0</v>
-      </c>
-      <c r="N22" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" t="s">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>0</v>
-      </c>
-      <c r="R22" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" t="s">
-        <v>0</v>
-      </c>
-      <c r="T22" t="s">
-        <v>0</v>
-      </c>
-      <c r="U22" t="s">
-        <v>0</v>
-      </c>
-      <c r="V22" t="s">
-        <v>0</v>
-      </c>
-      <c r="W22" t="s">
-        <v>0</v>
-      </c>
-      <c r="X22" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>0</v>
-      </c>
       <c r="AA22" t="s">
         <v>0</v>
       </c>
@@ -3229,6 +3207,9 @@
         <v>0</v>
       </c>
       <c r="AD22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE22" t="s">
         <v>0</v>
       </c>
       <c r="AH22" s="1"/>
@@ -3237,6 +3218,9 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
       <c r="E23" t="s">
         <v>0</v>
       </c>
@@ -3246,60 +3230,6 @@
       <c r="H23" t="s">
         <v>0</v>
       </c>
-      <c r="I23" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>0</v>
-      </c>
-      <c r="M23" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" t="s">
-        <v>0</v>
-      </c>
-      <c r="P23" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>0</v>
-      </c>
-      <c r="R23" t="s">
-        <v>0</v>
-      </c>
-      <c r="S23" t="s">
-        <v>0</v>
-      </c>
-      <c r="T23" t="s">
-        <v>0</v>
-      </c>
-      <c r="U23" t="s">
-        <v>0</v>
-      </c>
-      <c r="V23" t="s">
-        <v>0</v>
-      </c>
-      <c r="W23" t="s">
-        <v>0</v>
-      </c>
-      <c r="X23" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>0</v>
-      </c>
       <c r="AA23" t="s">
         <v>0</v>
       </c>
@@ -3307,6 +3237,9 @@
         <v>0</v>
       </c>
       <c r="AD23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE23" t="s">
         <v>0</v>
       </c>
       <c r="AH23" s="1"/>
@@ -3315,6 +3248,9 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
+      <c r="D24" t="s">
+        <v>0</v>
+      </c>
       <c r="E24" t="s">
         <v>0</v>
       </c>
@@ -3324,60 +3260,6 @@
       <c r="H24" t="s">
         <v>0</v>
       </c>
-      <c r="I24" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>0</v>
-      </c>
-      <c r="M24" t="s">
-        <v>0</v>
-      </c>
-      <c r="N24" t="s">
-        <v>0</v>
-      </c>
-      <c r="O24" t="s">
-        <v>0</v>
-      </c>
-      <c r="P24" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>0</v>
-      </c>
-      <c r="R24" t="s">
-        <v>0</v>
-      </c>
-      <c r="S24" t="s">
-        <v>0</v>
-      </c>
-      <c r="T24" t="s">
-        <v>0</v>
-      </c>
-      <c r="U24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V24" t="s">
-        <v>0</v>
-      </c>
-      <c r="W24" t="s">
-        <v>0</v>
-      </c>
-      <c r="X24" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>0</v>
-      </c>
       <c r="AA24" t="s">
         <v>0</v>
       </c>
@@ -3385,6 +3267,9 @@
         <v>0</v>
       </c>
       <c r="AD24" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE24" t="s">
         <v>0</v>
       </c>
       <c r="AH24" s="1"/>
@@ -3393,6 +3278,9 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
       <c r="E25" t="s">
         <v>0</v>
       </c>
@@ -3405,60 +3293,6 @@
       <c r="H25" t="s">
         <v>0</v>
       </c>
-      <c r="I25" t="s">
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>0</v>
-      </c>
-      <c r="M25" t="s">
-        <v>0</v>
-      </c>
-      <c r="N25" t="s">
-        <v>0</v>
-      </c>
-      <c r="O25" t="s">
-        <v>0</v>
-      </c>
-      <c r="P25" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>0</v>
-      </c>
-      <c r="R25" t="s">
-        <v>0</v>
-      </c>
-      <c r="S25" t="s">
-        <v>0</v>
-      </c>
-      <c r="T25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U25" t="s">
-        <v>0</v>
-      </c>
-      <c r="V25" t="s">
-        <v>0</v>
-      </c>
-      <c r="W25" t="s">
-        <v>0</v>
-      </c>
-      <c r="X25" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>0</v>
-      </c>
       <c r="AA25" t="s">
         <v>0</v>
       </c>
@@ -3469,6 +3303,9 @@
         <v>2</v>
       </c>
       <c r="AD25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="s">
         <v>0</v>
       </c>
       <c r="AH25" s="1"/>
@@ -3477,6 +3314,9 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
       <c r="E26" t="s">
         <v>0</v>
       </c>
@@ -3489,60 +3329,6 @@
       <c r="H26" t="s">
         <v>0</v>
       </c>
-      <c r="I26" t="s">
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" t="s">
-        <v>0</v>
-      </c>
-      <c r="N26" t="s">
-        <v>0</v>
-      </c>
-      <c r="O26" t="s">
-        <v>0</v>
-      </c>
-      <c r="P26" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>0</v>
-      </c>
-      <c r="R26" t="s">
-        <v>0</v>
-      </c>
-      <c r="S26" t="s">
-        <v>0</v>
-      </c>
-      <c r="T26" t="s">
-        <v>0</v>
-      </c>
-      <c r="U26" t="s">
-        <v>0</v>
-      </c>
-      <c r="V26" t="s">
-        <v>0</v>
-      </c>
-      <c r="W26" t="s">
-        <v>0</v>
-      </c>
-      <c r="X26" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>0</v>
-      </c>
       <c r="AA26" t="s">
         <v>0</v>
       </c>
@@ -3553,6 +3339,9 @@
         <v>0</v>
       </c>
       <c r="AD26" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE26" t="s">
         <v>0</v>
       </c>
       <c r="AH26" s="1"/>
@@ -3560,6 +3349,36 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>0</v>
       </c>
       <c r="AH27" s="1"/>
     </row>
@@ -3637,25 +3456,1777 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AG33">
+    <cfRule type="containsText" dxfId="48" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="4" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="5" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="6" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="7" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBD73F2-C36D-40BA-B5C4-271E35793465}">
+  <dimension ref="A1:AH34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>5</v>
+      </c>
+      <c r="T16" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" t="s">
+        <v>5</v>
+      </c>
+      <c r="T18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>0</v>
+      </c>
+      <c r="V19" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AH25" s="1"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="AH28" s="1"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH29" s="1"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="AH30" s="1"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="AH31" s="1"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="AH32" s="1"/>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH33" s="1"/>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:AG11 J12:AG14 B12:D14 D15:F16 R16:AG16 G15:AG15 B20:AG33 D17:AG19 C15:C19">
+    <cfRule type="containsText" dxfId="41" priority="8" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="9" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="10" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="11" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="13" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16:Q16">
+    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",G16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",G16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",G16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",G16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="5" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",G16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",G16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",G16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D63D92F-120A-4645-8B62-314493B95A80}">
+  <dimension ref="A1:AH34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="P9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="P10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="P11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="P12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="P13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="P14" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>0</v>
+      </c>
+      <c r="V14" t="s">
+        <v>6</v>
+      </c>
+      <c r="W14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="K16" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="W16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>0</v>
+      </c>
+      <c r="V17" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="K20" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="K22" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>6</v>
+      </c>
+      <c r="R22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AH25" s="1"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="AH28" s="1"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH29" s="1"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="AH30" s="1"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="AH31" s="1"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="AH32" s="1"/>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH33" s="1"/>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:AG14 J15:AG15 B15:H23 J18:J23 Q17:AG17 B25:AG33 B24:J24 Q18:Q22 R18:AG24 J16 L16:AG16 K16:K24 L23:Q24">
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:I23">
+    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",I15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",I15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",I15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",I15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",I15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",I15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",I15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17:P22">
     <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",L17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH("B",L17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",L17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",L17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",L17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",L17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",L17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B777CBD-ED7C-4D6D-8449-39F863820D08}">
+  <dimension ref="A1:AH34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AH25" s="1"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="AH28" s="1"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH29" s="1"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="AH30" s="1"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="AH31" s="1"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="AH32" s="1"/>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH33" s="1"/>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:AG33">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>